<commit_message>
Since both scanner and EEG computer mimic a keyboard, doKeyboard is made redundant. Changed all the functions that previousely used that option. Also got rid of other edudancies in options function
</commit_message>
<xml_diff>
--- a/control_task/+eventCreator/randomisation.xlsx
+++ b/control_task/+eventCreator/randomisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwellste/projects/SEPAB/tasks/social_affective_prediction_task/control_task/+eventCreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B40051E-4975-0C40-999F-B942708D1031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03434E96-87CC-0842-9F10-4920AAA16493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="1080" windowWidth="34560" windowHeight="18980" activeTab="2" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
+    <workbookView xWindow="32640" yWindow="1080" windowWidth="34560" windowHeight="18980" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
   </bookViews>
   <sheets>
     <sheet name="stimuli" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="17">
   <si>
     <t>f1</t>
   </si>
@@ -279,8 +279,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}" name="Table133" displayName="Table133" ref="A1:F42" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F42" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}" name="Table133" displayName="Table133" ref="A1:F43" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A1:F43" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{9D940E70-486F-1A48-B3BD-99EBD185807C}" name="PID" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{B417C134-6603-5943-A4A8-80D3A31FD98E}" name="practice_a1" dataDxfId="4"/>
@@ -603,9 +603,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A886A73D-7D5B-1440-9AEF-D5255F093359}">
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -639,7 +639,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1001</v>
+        <v>1999</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
@@ -656,804 +656,830 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F15" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E20" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F22" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E23" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F25" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E26" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="F26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F28" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F29" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F30" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F32" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1032</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>6</v>
+        <v>1031</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F33" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1033</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E34" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" t="s">
-        <v>3</v>
+        <v>1032</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F36" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E37" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C38" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E38" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F38" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E39" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F39" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F40" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C41" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
+        <v>1040</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>1</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E42" t="s">
+        <v>7</v>
+      </c>
+      <c r="F42" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>1041</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
-        <v>4</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E42" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="B43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2076,7 +2102,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67C183AB-8CD0-044E-A35E-D1387903F1DB}">
   <dimension ref="B3:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
amended task timings so that task is the same length even when participants miss a trial
</commit_message>
<xml_diff>
--- a/control_task/+eventCreator/randomisation.xlsx
+++ b/control_task/+eventCreator/randomisation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwellste/projects/SEPAB/tasks/social_affective_prediction_task/control_task/+eventCreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03434E96-87CC-0842-9F10-4920AAA16493}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF89C348-1B50-1F4C-BE51-CC5B7078E5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32640" yWindow="1080" windowWidth="34560" windowHeight="18980" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
   </bookViews>
   <sheets>
     <sheet name="stimuli" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="19">
   <si>
     <t>f1</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>AAA</t>
+  </si>
+  <si>
+    <t>patient</t>
+  </si>
+  <si>
+    <t>healthy</t>
   </si>
 </sst>
 </file>
@@ -173,18 +179,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -279,15 +302,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}" name="Table133" displayName="Table133" ref="A1:F43" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="A1:F43" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{9D940E70-486F-1A48-B3BD-99EBD185807C}" name="PID" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{B417C134-6603-5943-A4A8-80D3A31FD98E}" name="practice_a1" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{26478A98-03E6-704B-92AC-4812BFBB8EAD}" name="practice_a2" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{C6B2DDF5-D9D9-594E-986E-BE5AEEF133C8}" name="experiment_a1" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{F4A3FF6F-5F1A-8147-97FE-470CA83DA29C}" name="experiment_a2" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{050BCC80-4DC7-E44B-B335-32AAF61C00FF}" name="experiment_a3" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}" name="Table133" displayName="Table133" ref="A1:H44" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H44" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}"/>
+  <tableColumns count="8">
+    <tableColumn id="1" xr3:uid="{9D940E70-486F-1A48-B3BD-99EBD185807C}" name="PID" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{B417C134-6603-5943-A4A8-80D3A31FD98E}" name="practice_a1" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{26478A98-03E6-704B-92AC-4812BFBB8EAD}" name="practice_a2" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{C6B2DDF5-D9D9-594E-986E-BE5AEEF133C8}" name="experiment_a1" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F4A3FF6F-5F1A-8147-97FE-470CA83DA29C}" name="experiment_a2" dataDxfId="3"/>
+    <tableColumn id="8" xr3:uid="{050BCC80-4DC7-E44B-B335-32AAF61C00FF}" name="experiment_a3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{8F8F9FF5-1097-F24D-8F24-839DB3B3F4A6}" name="patient" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{7E5FABB7-CAC3-3E4F-9FF9-29742651D624}" name="healthy" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -603,15 +628,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A886A73D-7D5B-1440-9AEF-D5255F093359}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:O44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -630,14 +655,20 @@
       <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
+      <c r="G1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>18</v>
+      </c>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1999</v>
       </c>
@@ -656,830 +687,1114 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="G2" s="6">
+        <v>0</v>
+      </c>
+      <c r="H2" s="6">
+        <v>0</v>
+      </c>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>999</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4">
         <v>1001</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>1002</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="B5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>1003</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="B6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>1004</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="B7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>1005</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="B8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="6">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>1006</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>1007</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="B10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="6">
+        <v>0</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>1008</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>1009</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="6">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>1010</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E12" t="s">
-        <v>5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="B13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="6">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>1011</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>0</v>
-      </c>
-      <c r="F13" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="B14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="6">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>1012</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="B15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>1013</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E15" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="B16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="6">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>1014</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="B17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="6">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>1015</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="6">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>1016</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="6">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>1017</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" t="s">
-        <v>1</v>
-      </c>
-      <c r="F19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="B20" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="6">
+        <v>0</v>
+      </c>
+      <c r="H20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>1018</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" t="s">
-        <v>6</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="B21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>1019</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>1</v>
-      </c>
-      <c r="F21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="B22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="6">
+        <v>0</v>
+      </c>
+      <c r="H22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>1020</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23" s="6">
+        <v>0</v>
+      </c>
+      <c r="H23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>1021</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>7</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="B24" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>5</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>1022</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>1</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" t="s">
-        <v>2</v>
-      </c>
-      <c r="F24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="6">
+        <v>0</v>
+      </c>
+      <c r="H25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>1023</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E25" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="B26" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>5</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="6">
+        <v>0</v>
+      </c>
+      <c r="H26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>1024</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="B27" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>1025</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="B28" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G28" s="6">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>1026</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" t="s">
-        <v>6</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="B29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="6">
+        <v>0</v>
+      </c>
+      <c r="H29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>1027</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E29" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="B30" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0</v>
+      </c>
+      <c r="H30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>1028</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E30" t="s">
-        <v>5</v>
-      </c>
-      <c r="F30" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="B31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>5</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" s="6">
+        <v>0</v>
+      </c>
+      <c r="H31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>1029</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>2</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-      <c r="F31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="B32" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" t="s">
+        <v>3</v>
+      </c>
+      <c r="G32" s="6">
+        <v>0</v>
+      </c>
+      <c r="H32" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>1030</v>
       </c>
-      <c r="B32" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
-        <v>1</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="B33" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>0</v>
+      </c>
+      <c r="G33" s="6">
+        <v>0</v>
+      </c>
+      <c r="H33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>1031</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>0</v>
-      </c>
-      <c r="F33" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="B34" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" t="s">
+        <v>5</v>
+      </c>
+      <c r="G34" s="6">
+        <v>0</v>
+      </c>
+      <c r="H34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>1032</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
+      <c r="B35" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G35" s="6">
+        <v>0</v>
+      </c>
+      <c r="H35" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36">
         <v>1033</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E35" t="s">
-        <v>0</v>
-      </c>
-      <c r="F35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="B36" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>3</v>
+      </c>
+      <c r="G36" s="6">
+        <v>0</v>
+      </c>
+      <c r="H36" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>1034</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>5</v>
-      </c>
-      <c r="F36" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="B37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+      <c r="F37" t="s">
+        <v>0</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0</v>
+      </c>
+      <c r="H37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>1035</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" t="s">
-        <v>1</v>
-      </c>
-      <c r="F37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="B38" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1</v>
+      </c>
+      <c r="F38" t="s">
+        <v>5</v>
+      </c>
+      <c r="G38" s="6">
+        <v>0</v>
+      </c>
+      <c r="H38" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>1036</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>6</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" t="s">
-        <v>3</v>
-      </c>
-      <c r="F38" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="B39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>3</v>
+      </c>
+      <c r="F39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="6">
+        <v>0</v>
+      </c>
+      <c r="H39" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>1037</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E39" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="B40" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" t="s">
+        <v>7</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0</v>
+      </c>
+      <c r="H40" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41">
         <v>1038</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E40" t="s">
-        <v>2</v>
-      </c>
-      <c r="F40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="B41" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>2</v>
+      </c>
+      <c r="F41" t="s">
+        <v>4</v>
+      </c>
+      <c r="G41" s="6">
+        <v>0</v>
+      </c>
+      <c r="H41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42">
         <v>1039</v>
       </c>
-      <c r="B41" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" t="s">
-        <v>1</v>
-      </c>
-      <c r="F41" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
+      <c r="B42" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1</v>
+      </c>
+      <c r="F42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" s="6">
+        <v>0</v>
+      </c>
+      <c r="H42" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43">
         <v>1040</v>
       </c>
-      <c r="B42" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
-        <v>1</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E42" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
+      <c r="B43" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>7</v>
+      </c>
+      <c r="F43" t="s">
+        <v>6</v>
+      </c>
+      <c r="G43" s="6">
+        <v>0</v>
+      </c>
+      <c r="H43" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44">
         <v>1041</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
-        <v>4</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
+      <c r="B44" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>7</v>
+      </c>
+      <c r="F44" t="s">
+        <v>0</v>
+      </c>
+      <c r="G44" s="6">
+        <v>0</v>
+      </c>
+      <c r="H44" s="6">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added EMG triggers and functions to send triggers to BrainVision
</commit_message>
<xml_diff>
--- a/control_task/+eventCreator/randomisation.xlsx
+++ b/control_task/+eventCreator/randomisation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwellste/projects/SEPAB/tasks/social_affective_prediction_task/control_task/+eventCreator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF89C348-1B50-1F4C-BE51-CC5B7078E5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31FCFD5F-A157-4F4B-9AAC-22FDB995E561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="1" xr2:uid="{960645DE-D3B2-7545-8897-4998A9B98D00}"/>
   </bookViews>
   <sheets>
     <sheet name="stimuli" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="19">
   <si>
     <t>f1</t>
   </si>
@@ -179,7 +179,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -187,6 +187,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -302,8 +305,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}" name="Table133" displayName="Table133" ref="A1:H44" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A1:H44" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}" name="Table133" displayName="Table133" ref="A1:H85" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A1:H85" xr:uid="{F67422B3-C14F-0041-8814-6319BB48511E}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{9D940E70-486F-1A48-B3BD-99EBD185807C}" name="PID" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{B417C134-6603-5943-A4A8-80D3A31FD98E}" name="practice_a1" dataDxfId="6"/>
@@ -319,8 +322,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61FB41AB-D6DC-B04E-BF97-58A9E1B06495}" name="Table2" displayName="Table2" ref="A1:D42" totalsRowShown="0">
-  <autoFilter ref="A1:D42" xr:uid="{61FB41AB-D6DC-B04E-BF97-58A9E1B06495}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61FB41AB-D6DC-B04E-BF97-58A9E1B06495}" name="Table2" displayName="Table2" ref="A1:D83" totalsRowShown="0">
+  <autoFilter ref="A1:D83" xr:uid="{61FB41AB-D6DC-B04E-BF97-58A9E1B06495}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{4673DE77-AD88-9F49-95CD-81209C726E34}" name="PID"/>
     <tableColumn id="2" xr3:uid="{E700E40E-65BA-7441-BAC6-4EF8EC301B17}" name="SAP"/>
@@ -628,10 +631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A886A73D-7D5B-1440-9AEF-D5255F093359}">
-  <dimension ref="A1:O44"/>
+  <dimension ref="A1:O85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="J70" sqref="J70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -655,10 +658,10 @@
       <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="J1" s="5"/>
@@ -687,10 +690,10 @@
       <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="6">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
       <c r="J2" s="5"/>
@@ -719,10 +722,10 @@
       <c r="F3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
       <c r="J3" s="5"/>
@@ -751,10 +754,10 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="6">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>0</v>
       </c>
     </row>
@@ -777,10 +780,10 @@
       <c r="F5" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>0</v>
       </c>
     </row>
@@ -803,10 +806,10 @@
       <c r="F6" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>0</v>
       </c>
     </row>
@@ -829,10 +832,10 @@
       <c r="F7" t="s">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>
@@ -855,10 +858,10 @@
       <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="6">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>0</v>
       </c>
     </row>
@@ -881,10 +884,10 @@
       <c r="F9" t="s">
         <v>6</v>
       </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>0</v>
       </c>
     </row>
@@ -907,10 +910,10 @@
       <c r="F10" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>0</v>
       </c>
     </row>
@@ -933,10 +936,10 @@
       <c r="F11" t="s">
         <v>4</v>
       </c>
-      <c r="G11" s="6">
-        <v>0</v>
-      </c>
-      <c r="H11" s="6">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>0</v>
       </c>
     </row>
@@ -959,10 +962,10 @@
       <c r="F12" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="6">
-        <v>0</v>
-      </c>
-      <c r="H12" s="6">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>0</v>
       </c>
     </row>
@@ -985,10 +988,10 @@
       <c r="F13" t="s">
         <v>6</v>
       </c>
-      <c r="G13" s="6">
-        <v>0</v>
-      </c>
-      <c r="H13" s="6">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>0</v>
       </c>
     </row>
@@ -1011,10 +1014,10 @@
       <c r="F14" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="6">
-        <v>0</v>
-      </c>
-      <c r="H14" s="6">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>0</v>
       </c>
     </row>
@@ -1037,10 +1040,10 @@
       <c r="F15" t="s">
         <v>1</v>
       </c>
-      <c r="G15" s="6">
-        <v>0</v>
-      </c>
-      <c r="H15" s="6">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>0</v>
       </c>
     </row>
@@ -1063,10 +1066,10 @@
       <c r="F16" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="6">
-        <v>0</v>
-      </c>
-      <c r="H16" s="6">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>0</v>
       </c>
     </row>
@@ -1089,10 +1092,10 @@
       <c r="F17" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="6">
-        <v>0</v>
-      </c>
-      <c r="H17" s="6">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>0</v>
       </c>
     </row>
@@ -1115,10 +1118,10 @@
       <c r="F18" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="6">
-        <v>0</v>
-      </c>
-      <c r="H18" s="6">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>0</v>
       </c>
     </row>
@@ -1141,10 +1144,10 @@
       <c r="F19" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="6">
-        <v>0</v>
-      </c>
-      <c r="H19" s="6">
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
         <v>0</v>
       </c>
     </row>
@@ -1167,10 +1170,10 @@
       <c r="F20" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="6">
-        <v>0</v>
-      </c>
-      <c r="H20" s="6">
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
         <v>0</v>
       </c>
     </row>
@@ -1193,10 +1196,10 @@
       <c r="F21" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="6">
-        <v>0</v>
-      </c>
-      <c r="H21" s="6">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
         <v>0</v>
       </c>
     </row>
@@ -1219,10 +1222,10 @@
       <c r="F22" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="6">
-        <v>0</v>
-      </c>
-      <c r="H22" s="6">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
         <v>0</v>
       </c>
     </row>
@@ -1245,10 +1248,10 @@
       <c r="F23" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="6">
-        <v>0</v>
-      </c>
-      <c r="H23" s="6">
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
         <v>0</v>
       </c>
     </row>
@@ -1271,10 +1274,10 @@
       <c r="F24" t="s">
         <v>5</v>
       </c>
-      <c r="G24" s="6">
-        <v>0</v>
-      </c>
-      <c r="H24" s="6">
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
         <v>0</v>
       </c>
     </row>
@@ -1297,10 +1300,10 @@
       <c r="F25" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="6">
-        <v>0</v>
-      </c>
-      <c r="H25" s="6">
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
         <v>0</v>
       </c>
     </row>
@@ -1323,10 +1326,10 @@
       <c r="F26" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="6">
-        <v>0</v>
-      </c>
-      <c r="H26" s="6">
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
         <v>0</v>
       </c>
     </row>
@@ -1349,10 +1352,10 @@
       <c r="F27" t="s">
         <v>1</v>
       </c>
-      <c r="G27" s="6">
-        <v>0</v>
-      </c>
-      <c r="H27" s="6">
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="H27">
         <v>0</v>
       </c>
     </row>
@@ -1375,10 +1378,10 @@
       <c r="F28" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="6">
-        <v>0</v>
-      </c>
-      <c r="H28" s="6">
+      <c r="G28">
+        <v>0</v>
+      </c>
+      <c r="H28">
         <v>0</v>
       </c>
     </row>
@@ -1401,10 +1404,10 @@
       <c r="F29" t="s">
         <v>4</v>
       </c>
-      <c r="G29" s="6">
-        <v>0</v>
-      </c>
-      <c r="H29" s="6">
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="H29">
         <v>0</v>
       </c>
     </row>
@@ -1427,10 +1430,10 @@
       <c r="F30" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="6">
-        <v>0</v>
-      </c>
-      <c r="H30" s="6">
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="H30">
         <v>0</v>
       </c>
     </row>
@@ -1453,10 +1456,10 @@
       <c r="F31" t="s">
         <v>1</v>
       </c>
-      <c r="G31" s="6">
-        <v>0</v>
-      </c>
-      <c r="H31" s="6">
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
         <v>0</v>
       </c>
     </row>
@@ -1479,10 +1482,10 @@
       <c r="F32" t="s">
         <v>3</v>
       </c>
-      <c r="G32" s="6">
-        <v>0</v>
-      </c>
-      <c r="H32" s="6">
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
         <v>0</v>
       </c>
     </row>
@@ -1505,10 +1508,10 @@
       <c r="F33" t="s">
         <v>0</v>
       </c>
-      <c r="G33" s="6">
-        <v>0</v>
-      </c>
-      <c r="H33" s="6">
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
         <v>0</v>
       </c>
     </row>
@@ -1531,10 +1534,10 @@
       <c r="F34" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="6">
-        <v>0</v>
-      </c>
-      <c r="H34" s="6">
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
         <v>0</v>
       </c>
     </row>
@@ -1557,10 +1560,10 @@
       <c r="F35" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G35" s="6">
-        <v>0</v>
-      </c>
-      <c r="H35" s="6">
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
         <v>0</v>
       </c>
     </row>
@@ -1583,10 +1586,10 @@
       <c r="F36" t="s">
         <v>3</v>
       </c>
-      <c r="G36" s="6">
-        <v>0</v>
-      </c>
-      <c r="H36" s="6">
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
         <v>0</v>
       </c>
     </row>
@@ -1609,10 +1612,10 @@
       <c r="F37" t="s">
         <v>0</v>
       </c>
-      <c r="G37" s="6">
-        <v>0</v>
-      </c>
-      <c r="H37" s="6">
+      <c r="G37">
+        <v>0</v>
+      </c>
+      <c r="H37">
         <v>0</v>
       </c>
     </row>
@@ -1635,10 +1638,10 @@
       <c r="F38" t="s">
         <v>5</v>
       </c>
-      <c r="G38" s="6">
-        <v>0</v>
-      </c>
-      <c r="H38" s="6">
+      <c r="G38">
+        <v>0</v>
+      </c>
+      <c r="H38">
         <v>0</v>
       </c>
     </row>
@@ -1661,10 +1664,10 @@
       <c r="F39" t="s">
         <v>1</v>
       </c>
-      <c r="G39" s="6">
-        <v>0</v>
-      </c>
-      <c r="H39" s="6">
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
         <v>0</v>
       </c>
     </row>
@@ -1687,10 +1690,10 @@
       <c r="F40" t="s">
         <v>7</v>
       </c>
-      <c r="G40" s="6">
-        <v>0</v>
-      </c>
-      <c r="H40" s="6">
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
         <v>0</v>
       </c>
     </row>
@@ -1713,10 +1716,10 @@
       <c r="F41" t="s">
         <v>4</v>
       </c>
-      <c r="G41" s="6">
-        <v>0</v>
-      </c>
-      <c r="H41" s="6">
+      <c r="G41">
+        <v>0</v>
+      </c>
+      <c r="H41">
         <v>0</v>
       </c>
     </row>
@@ -1739,10 +1742,10 @@
       <c r="F42" t="s">
         <v>2</v>
       </c>
-      <c r="G42" s="6">
-        <v>0</v>
-      </c>
-      <c r="H42" s="6">
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
         <v>0</v>
       </c>
     </row>
@@ -1765,10 +1768,10 @@
       <c r="F43" t="s">
         <v>6</v>
       </c>
-      <c r="G43" s="6">
-        <v>0</v>
-      </c>
-      <c r="H43" s="6">
+      <c r="G43">
+        <v>0</v>
+      </c>
+      <c r="H43">
         <v>0</v>
       </c>
     </row>
@@ -1791,10 +1794,1076 @@
       <c r="F44" t="s">
         <v>0</v>
       </c>
-      <c r="G44" s="6">
-        <v>0</v>
-      </c>
-      <c r="H44" s="6">
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="6">
+        <v>2001</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G45" s="6">
+        <v>0</v>
+      </c>
+      <c r="H45" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="6">
+        <v>2002</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G46" s="6">
+        <v>0</v>
+      </c>
+      <c r="H46" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="6">
+        <v>2003</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D47" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G47" s="6">
+        <v>0</v>
+      </c>
+      <c r="H47" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="6">
+        <v>2004</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G48" s="6">
+        <v>0</v>
+      </c>
+      <c r="H48" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="6">
+        <v>2005</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G49" s="6">
+        <v>0</v>
+      </c>
+      <c r="H49" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="6">
+        <v>2006</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" s="6">
+        <v>0</v>
+      </c>
+      <c r="H50" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="6">
+        <v>2007</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G51" s="6">
+        <v>0</v>
+      </c>
+      <c r="H51" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="6">
+        <v>2008</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="6">
+        <v>0</v>
+      </c>
+      <c r="H52" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="6">
+        <v>2009</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="6">
+        <v>0</v>
+      </c>
+      <c r="H53" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="6">
+        <v>2010</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="6">
+        <v>0</v>
+      </c>
+      <c r="H54" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>2011</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G55" s="6">
+        <v>0</v>
+      </c>
+      <c r="H55" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>2012</v>
+      </c>
+      <c r="B56" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G56" s="6">
+        <v>0</v>
+      </c>
+      <c r="H56" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="6">
+        <v>2013</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C57" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G57" s="6">
+        <v>0</v>
+      </c>
+      <c r="H57" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="6">
+        <v>2014</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F58" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="6">
+        <v>0</v>
+      </c>
+      <c r="H58" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="6">
+        <v>2015</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G59" s="6">
+        <v>0</v>
+      </c>
+      <c r="H59" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="6">
+        <v>2016</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C60" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F60" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="6">
+        <v>0</v>
+      </c>
+      <c r="H60" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="6">
+        <v>2017</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G61" s="6">
+        <v>0</v>
+      </c>
+      <c r="H61" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="6">
+        <v>2018</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E62" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F62" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G62" s="6">
+        <v>0</v>
+      </c>
+      <c r="H62" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="6">
+        <v>2019</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F63" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G63" s="6">
+        <v>0</v>
+      </c>
+      <c r="H63" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="6">
+        <v>2020</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F64" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="6">
+        <v>0</v>
+      </c>
+      <c r="H64" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="6">
+        <v>2021</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G65" s="6">
+        <v>0</v>
+      </c>
+      <c r="H65" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="6">
+        <v>2022</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="6">
+        <v>0</v>
+      </c>
+      <c r="H66" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="6">
+        <v>2023</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F67" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G67" s="6">
+        <v>0</v>
+      </c>
+      <c r="H67" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="6">
+        <v>2024</v>
+      </c>
+      <c r="B68" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G68" s="6">
+        <v>0</v>
+      </c>
+      <c r="H68" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="6">
+        <v>2025</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C69" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E69" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F69" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G69" s="6">
+        <v>0</v>
+      </c>
+      <c r="H69" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="6">
+        <v>2026</v>
+      </c>
+      <c r="B70" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C70" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E70" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F70" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="6">
+        <v>0</v>
+      </c>
+      <c r="H70" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="6">
+        <v>2027</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C71" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F71" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G71" s="6">
+        <v>0</v>
+      </c>
+      <c r="H71" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="6">
+        <v>2028</v>
+      </c>
+      <c r="B72" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G72" s="6">
+        <v>0</v>
+      </c>
+      <c r="H72" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="6">
+        <v>2029</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C73" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D73" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G73" s="6">
+        <v>0</v>
+      </c>
+      <c r="H73" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="6">
+        <v>2030</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D74" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F74" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G74" s="6">
+        <v>0</v>
+      </c>
+      <c r="H74" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="6">
+        <v>2031</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G75" s="6">
+        <v>0</v>
+      </c>
+      <c r="H75" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="6">
+        <v>2032</v>
+      </c>
+      <c r="B76" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G76" s="6">
+        <v>0</v>
+      </c>
+      <c r="H76" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="6">
+        <v>2033</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F77" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G77" s="6">
+        <v>0</v>
+      </c>
+      <c r="H77" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="6">
+        <v>2034</v>
+      </c>
+      <c r="B78" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G78" s="6">
+        <v>0</v>
+      </c>
+      <c r="H78" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="6">
+        <v>2035</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F79" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G79" s="6">
+        <v>0</v>
+      </c>
+      <c r="H79" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="6">
+        <v>2036</v>
+      </c>
+      <c r="B80" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F80" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G80" s="6">
+        <v>0</v>
+      </c>
+      <c r="H80" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="6">
+        <v>2037</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F81" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G81" s="6">
+        <v>0</v>
+      </c>
+      <c r="H81" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="6">
+        <v>2038</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E82" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F82" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G82" s="6">
+        <v>0</v>
+      </c>
+      <c r="H82" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="6">
+        <v>2039</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D83" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F83" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G83" s="6">
+        <v>0</v>
+      </c>
+      <c r="H83" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="6">
+        <v>2040</v>
+      </c>
+      <c r="B84" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D84" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E84" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F84" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G84" s="6">
+        <v>0</v>
+      </c>
+      <c r="H84" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="6">
+        <v>2041</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F85" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="G85" s="6">
+        <v>0</v>
+      </c>
+      <c r="H85" s="6">
         <v>0</v>
       </c>
     </row>
@@ -1809,10 +2878,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3200B542-BDCF-2745-BDDC-EAB97779DBE2}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="G72" sqref="G72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2402,6 +3471,580 @@
         <v>2</v>
       </c>
       <c r="D42">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>2001</v>
+      </c>
+      <c r="B43">
+        <v>1</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>2002</v>
+      </c>
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2003</v>
+      </c>
+      <c r="B45">
+        <v>1</v>
+      </c>
+      <c r="C45">
+        <v>2</v>
+      </c>
+      <c r="D45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2004</v>
+      </c>
+      <c r="B46">
+        <v>2</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2005</v>
+      </c>
+      <c r="B47">
+        <v>1</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2006</v>
+      </c>
+      <c r="B48">
+        <v>2</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2007</v>
+      </c>
+      <c r="B49">
+        <v>1</v>
+      </c>
+      <c r="C49">
+        <v>2</v>
+      </c>
+      <c r="D49">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2008</v>
+      </c>
+      <c r="B50">
+        <v>2</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2009</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>2</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2010</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2011</v>
+      </c>
+      <c r="B53">
+        <v>1</v>
+      </c>
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>2012</v>
+      </c>
+      <c r="B54">
+        <v>2</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>2013</v>
+      </c>
+      <c r="B55">
+        <v>1</v>
+      </c>
+      <c r="C55">
+        <v>2</v>
+      </c>
+      <c r="D55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>2014</v>
+      </c>
+      <c r="B56">
+        <v>2</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>2015</v>
+      </c>
+      <c r="B57">
+        <v>1</v>
+      </c>
+      <c r="C57">
+        <v>2</v>
+      </c>
+      <c r="D57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>2016</v>
+      </c>
+      <c r="B58">
+        <v>2</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>2017</v>
+      </c>
+      <c r="B59">
+        <v>1</v>
+      </c>
+      <c r="C59">
+        <v>2</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>2018</v>
+      </c>
+      <c r="B60">
+        <v>2</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2019</v>
+      </c>
+      <c r="B61">
+        <v>1</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+      <c r="D61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2020</v>
+      </c>
+      <c r="B62">
+        <v>2</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2021</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63">
+        <v>2</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2022</v>
+      </c>
+      <c r="B64">
+        <v>2</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
+      </c>
+      <c r="D64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>2023</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>2</v>
+      </c>
+      <c r="D65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>2024</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>2025</v>
+      </c>
+      <c r="B67">
+        <v>1</v>
+      </c>
+      <c r="C67">
+        <v>2</v>
+      </c>
+      <c r="D67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>2026</v>
+      </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>1</v>
+      </c>
+      <c r="D68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>2027</v>
+      </c>
+      <c r="B69">
+        <v>1</v>
+      </c>
+      <c r="C69">
+        <v>2</v>
+      </c>
+      <c r="D69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>2028</v>
+      </c>
+      <c r="B70">
+        <v>2</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2029</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>2030</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <v>1</v>
+      </c>
+      <c r="D72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>2031</v>
+      </c>
+      <c r="B73">
+        <v>1</v>
+      </c>
+      <c r="C73">
+        <v>2</v>
+      </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>2032</v>
+      </c>
+      <c r="B74">
+        <v>2</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>2033</v>
+      </c>
+      <c r="B75">
+        <v>1</v>
+      </c>
+      <c r="C75">
+        <v>2</v>
+      </c>
+      <c r="D75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>2034</v>
+      </c>
+      <c r="B76">
+        <v>2</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+      <c r="D76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>2035</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>2</v>
+      </c>
+      <c r="D77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>2036</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+      <c r="D78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2037</v>
+      </c>
+      <c r="B79">
+        <v>1</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+      <c r="D79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2038</v>
+      </c>
+      <c r="B80">
+        <v>2</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+      <c r="D80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>2039</v>
+      </c>
+      <c r="B81">
+        <v>1</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+      <c r="D81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2040</v>
+      </c>
+      <c r="B82">
+        <v>2</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>2041</v>
+      </c>
+      <c r="B83">
+        <v>1</v>
+      </c>
+      <c r="C83">
+        <v>2</v>
+      </c>
+      <c r="D83">
         <v>3</v>
       </c>
     </row>

</xml_diff>